<commit_message>
Adiciona suporte a células do tipo Boolean no importador de planilhas do Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/importer/multi_types.xlsx
+++ b/src/test/resources/importer/multi_types.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="25600" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NAME</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
   </si>
 </sst>
 </file>
@@ -41,7 +44,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -49,7 +52,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -87,8 +89,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,11 +422,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -432,7 +432,7 @@
     <col min="4" max="4" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +445,11 @@
       <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -458,6 +461,9 @@
       </c>
       <c r="D2" s="5">
         <v>1500.5</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>